<commit_message>
Collected historic data and created email function
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -15,7 +15,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -45,12 +48,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -124,10 +134,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Crypto_prices" displayName="Crypto_prices" ref="A1:G2" headerRowCount="1">
-  <autoFilter ref="A1:G3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Árak" displayName="Crypto_prices" ref="A1:G7" headerRowCount="1">
+  <autoFilter ref="A1:G2"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Dátum"/>
+    <tableColumn id="1" name="Dátum" dataDxfId="0"/>
     <tableColumn id="2" name="Ethereum"/>
     <tableColumn id="3" name="BNB"/>
     <tableColumn id="4" name="Cardano"/>
@@ -428,13 +438,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="10.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -474,28 +487,141 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2021/08/19</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>44395</v>
       </c>
       <c r="B2" t="n">
-        <v>2999.6</v>
+        <v>1900</v>
       </c>
       <c r="C2" t="n">
-        <v>403.47</v>
+        <v>301</v>
       </c>
       <c r="D2" t="n">
-        <v>2.11</v>
+        <v>1.18</v>
       </c>
       <c r="E2" t="n">
-        <v>1.13</v>
+        <v>0.59</v>
       </c>
       <c r="F2" t="n">
-        <v>0.11716</v>
+        <v>0.06569999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>3.27</v>
+        <v>2.01</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>44402</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2184</v>
+      </c>
+      <c r="C3" t="n">
+        <v>301</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0723</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.05</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>44409</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2542</v>
+      </c>
+      <c r="C4" t="n">
+        <v>335</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0897</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>44416</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3151</v>
+      </c>
+      <c r="C5" t="n">
+        <v>356</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1037</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>44423</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3269</v>
+      </c>
+      <c r="C6" t="n">
+        <v>409</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1305</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>44430</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3224</v>
+      </c>
+      <c r="C7" t="n">
+        <v>450</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>